<commit_message>
added dummy contents for mainLayout. Will experiment on hiding it on zoom next session
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13FB2A8-E1CA-4326-A08C-91F356E78B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD98DAC-F170-4B4E-90DF-84965C7F61D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Task</t>
   </si>
@@ -46,16 +46,40 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Task 1: Footer below that auto adjusts on zoom levels</t>
-  </si>
-  <si>
     <t>In Development</t>
   </si>
   <si>
-    <t>Task 2:</t>
-  </si>
-  <si>
     <t>Sm:mt-12 md:mt-14 lg:24 for its margins mayb</t>
+  </si>
+  <si>
+    <t>Task 2: Home Page that auto adjusts on zoom levels</t>
+  </si>
+  <si>
+    <t>Task 1: Layout including footer and header that auto adjusts on zoom levels</t>
+  </si>
+  <si>
+    <t>Task 3:</t>
+  </si>
+  <si>
+    <t>Task 4:</t>
+  </si>
+  <si>
+    <t>Task 5:</t>
+  </si>
+  <si>
+    <t>Task 6:</t>
+  </si>
+  <si>
+    <t>Task 7:</t>
+  </si>
+  <si>
+    <t>Task 8:</t>
+  </si>
+  <si>
+    <t>Task 9:</t>
+  </si>
+  <si>
+    <t>Task 10:</t>
   </si>
 </sst>
 </file>
@@ -427,20 +451,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="62.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,20 +475,63 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Homepage, added login and register buttons
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD98DAC-F170-4B4E-90DF-84965C7F61D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329BEC41-95A3-437C-AA1E-1FE9A004C2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Task</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>In Development</t>
-  </si>
-  <si>
     <t>Sm:mt-12 md:mt-14 lg:24 for its margins mayb</t>
   </si>
   <si>
@@ -58,18 +55,6 @@
     <t>Task 1: Layout including footer and header that auto adjusts on zoom levels</t>
   </si>
   <si>
-    <t>Task 3:</t>
-  </si>
-  <si>
-    <t>Task 4:</t>
-  </si>
-  <si>
-    <t>Task 5:</t>
-  </si>
-  <si>
-    <t>Task 6:</t>
-  </si>
-  <si>
     <t>Task 7:</t>
   </si>
   <si>
@@ -80,14 +65,46 @@
   </si>
   <si>
     <t>Task 10:</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>01/30/2024</t>
+  </si>
+  <si>
+    <t>Date Last Updated</t>
+  </si>
+  <si>
+    <t>using max-width min-width on css to make it so</t>
+  </si>
+  <si>
+    <t>Task 3: Login Page</t>
+  </si>
+  <si>
+    <t>Task 4: Establish DB Env</t>
+  </si>
+  <si>
+    <t>Task 5: DB:Schema</t>
+  </si>
+  <si>
+    <t>Task 6: Create Necessary DB Tables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -115,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,90 +469,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="62.109375" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added defineemits and props to homepage to trigger loginmodal
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329BEC41-95A3-437C-AA1E-1FE9A004C2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF54E96-7A28-495D-B4AB-6580A8E1BEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Task 1: Layout including footer and header that auto adjusts on zoom levels</t>
   </si>
   <si>
-    <t>Task 7:</t>
-  </si>
-  <si>
     <t>Task 8:</t>
   </si>
   <si>
@@ -79,23 +76,35 @@
     <t>using max-width min-width on css to make it so</t>
   </si>
   <si>
-    <t>Task 3: Login Page</t>
-  </si>
-  <si>
-    <t>Task 4: Establish DB Env</t>
-  </si>
-  <si>
-    <t>Task 5: DB:Schema</t>
-  </si>
-  <si>
-    <t>Task 6: Create Necessary DB Tables</t>
+    <t>Task 7:Create Necessary DB Tables</t>
+  </si>
+  <si>
+    <t>Task 6: DB:Schema</t>
+  </si>
+  <si>
+    <t>Task 5: Establish DB Env</t>
+  </si>
+  <si>
+    <t>Task 4: Login Page/Modal</t>
+  </si>
+  <si>
+    <t>Task 3: Register Page/Modal</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>polishing UI Design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +116,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,9 +157,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,75 +522,135 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45324</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added login modal with complete UI design
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF54E96-7A28-495D-B4AB-6580A8E1BEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A70D43-95D8-41A8-9EA5-92A44F238A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Task</t>
   </si>
@@ -85,26 +85,29 @@
     <t>Task 5: Establish DB Env</t>
   </si>
   <si>
-    <t>Task 4: Login Page/Modal</t>
-  </si>
-  <si>
-    <t>Task 3: Register Page/Modal</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
     <t>polishing UI Design</t>
+  </si>
+  <si>
+    <t>Task 4: Login Modal</t>
+  </si>
+  <si>
+    <t>Task 3: Register Page</t>
+  </si>
+  <si>
+    <t>In Development</t>
+  </si>
+  <si>
+    <t>Status Types</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,7 +134,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B0F0"/>
+      <color theme="7"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,12 +168,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,9 +523,11 @@
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="62.140625" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,8 +540,11 @@
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -538,8 +557,11 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -552,105 +574,114 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45324</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>45324</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added another blank modal for register feature
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A70D43-95D8-41A8-9EA5-92A44F238A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E04504-BE7E-4DD6-9C9F-40D24DEB2056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -55,12 +55,6 @@
     <t>Task 1: Layout including footer and header that auto adjusts on zoom levels</t>
   </si>
   <si>
-    <t>Task 8:</t>
-  </si>
-  <si>
-    <t>Task 9:</t>
-  </si>
-  <si>
     <t>Task 10:</t>
   </si>
   <si>
@@ -101,6 +95,12 @@
   </si>
   <si>
     <t>Status Types</t>
+  </si>
+  <si>
+    <t>Task 8: Login Backend</t>
+  </si>
+  <si>
+    <t>Task 9: Register Backend</t>
   </si>
 </sst>
 </file>
@@ -511,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +527,7 @@
     <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,150 +538,150 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3">
         <v>45324</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3">
         <v>45324</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed docker rootnode bug & configured env (also updated erd, to create tables tomorrow)
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4314D91-CE5E-4F50-90A0-C554F5D2309A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFB4DB4-322F-4CA8-BF0F-70D20FCEEB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,16 +634,16 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added projects controller, factory, model, and migration
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFB4DB4-322F-4CA8-BF0F-70D20FCEEB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265134D-6573-4AD5-8482-D8E2F0BD707A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -76,27 +76,18 @@
     <t>Task 4: Login Modal</t>
   </si>
   <si>
-    <t>Task 3: Register Page</t>
-  </si>
-  <si>
     <t>In Development</t>
   </si>
   <si>
     <t>Status Types</t>
   </si>
   <si>
-    <t>Task 8: Login Backend</t>
-  </si>
-  <si>
     <t>Task 9: Register Backend</t>
   </si>
   <si>
     <t>Backend part remaining</t>
   </si>
   <si>
-    <t>Task 11:</t>
-  </si>
-  <si>
     <t>Task 12:</t>
   </si>
   <si>
@@ -122,6 +113,15 @@
   </si>
   <si>
     <t>Task 7:Create DB Tables</t>
+  </si>
+  <si>
+    <t>Task 11: Login Backend</t>
+  </si>
+  <si>
+    <t>Task 8: Create Factory for dummy data</t>
+  </si>
+  <si>
+    <t>Task 3: Register Modal</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -596,21 +596,21 @@
         <v>7</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3">
-        <v>45324</v>
+        <v>45414</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>11</v>
@@ -624,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3">
         <v>45324</v>
@@ -637,26 +637,32 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D6" s="3">
+        <v>45445</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D7" s="3">
+        <v>45445</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>11</v>
@@ -664,7 +670,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
@@ -672,7 +678,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
@@ -680,7 +686,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>11</v>
@@ -688,7 +694,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -696,7 +702,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -704,7 +710,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
@@ -712,7 +718,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
@@ -720,7 +726,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -728,7 +734,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added factory for dem tables
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265134D-6573-4AD5-8482-D8E2F0BD707A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824A67B9-F027-4C98-AF55-A3FD4419A943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>Task 4: Login Modal</t>
-  </si>
-  <si>
     <t>In Development</t>
   </si>
   <si>
@@ -121,7 +118,10 @@
     <t>Task 8: Create Factory for dummy data</t>
   </si>
   <si>
-    <t>Task 3: Register Modal</t>
+    <t>Task 3: Login Modal</t>
+  </si>
+  <si>
+    <t>Task 4: Register Modal</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -596,21 +596,21 @@
         <v>7</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3">
-        <v>45414</v>
+        <v>45324</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>11</v>
@@ -618,16 +618,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3">
-        <v>45324</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -654,23 +654,29 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45475</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45475</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
@@ -678,7 +684,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
@@ -686,7 +692,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>11</v>
@@ -694,7 +700,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -702,7 +708,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -710,7 +716,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
@@ -718,7 +724,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
@@ -726,7 +732,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -734,7 +740,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
established route for register, syntax is new btw
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824A67B9-F027-4C98-AF55-A3FD4419A943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9994370-3DD4-47C2-835D-923B3E89B3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,8 +678,8 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added backend for register, but having trouble with reflecting auth on layout page
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9994370-3DD4-47C2-835D-923B3E89B3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA78449-38C9-422C-B573-053C5A8B4665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Task 4: Register Modal</t>
+  </si>
+  <si>
+    <t>Having a problem with reflecting auth frontend</t>
+  </si>
+  <si>
+    <t>02/13/2024</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,6 +687,12 @@
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
configured required inputs for register field, needs frontend message error to show when misinput occurs
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA78449-38C9-422C-B573-053C5A8B4665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D39C1DD-DBAD-489B-AE38-BA1454915383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>Backend part remaining</t>
   </si>
   <si>
-    <t>Task 12:</t>
-  </si>
-  <si>
     <t>Task 13:</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Task 7:Create DB Tables</t>
   </si>
   <si>
-    <t>Task 11: Login Backend</t>
-  </si>
-  <si>
     <t>Task 8: Create Factory for dummy data</t>
   </si>
   <si>
@@ -124,10 +118,16 @@
     <t>Task 4: Register Modal</t>
   </si>
   <si>
-    <t>Having a problem with reflecting auth frontend</t>
-  </si>
-  <si>
-    <t>02/13/2024</t>
+    <t>regsiter backend complete, needs error message to refleft when misinput</t>
+  </si>
+  <si>
+    <t>02/14/2024</t>
+  </si>
+  <si>
+    <t>Task 11: Logout Backend</t>
+  </si>
+  <si>
+    <t>Task 12 :Login Backend</t>
   </si>
 </sst>
 </file>
@@ -541,14 +541,14 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
@@ -607,7 +607,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
@@ -688,15 +688,15 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>11</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -720,7 +720,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
@@ -736,7 +736,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed register modal not closing after successfully registering after submitting field misinput
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49650845-B20D-4F82-A75B-732EE34FBC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3700389E-0E47-4761-8372-0D0F7904CAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -127,10 +127,11 @@
     <t>02/15/2024</t>
   </si>
   <si>
-    <t>register backend complete, needs error message to refleft when misinput</t>
-  </si>
-  <si>
     <t>02/16/2024</t>
+  </si>
+  <si>
+    <t>not sure if this is complete yet, but it seems it is. Had an issue where 
+modal wasn’t closing after form misinput</t>
   </si>
 </sst>
 </file>
@@ -198,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -207,6 +208,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +548,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,15 +687,15 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
@@ -705,15 +709,18 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added complete login feature, to tweak its UI next session
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3700389E-0E47-4761-8372-0D0F7904CAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8210987B-8502-4D66-83CC-2428A32C0699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -132,6 +132,12 @@
   <si>
     <t>not sure if this is complete yet, but it seems it is. Had an issue where 
 modal wasn’t closing after form misinput</t>
+  </si>
+  <si>
+    <t>after implementing this, a bug where flash msg persists appeared</t>
+  </si>
+  <si>
+    <t>Register, logout, and login has a flash bug, and its error msg needs revamp</t>
   </si>
 </sst>
 </file>
@@ -547,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,8 +697,8 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>31</v>
@@ -705,8 +711,11 @@
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
@@ -718,6 +727,9 @@
       </c>
       <c r="B12" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
fixed flash success not fading out after login/logout bug
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8210987B-8502-4D66-83CC-2428A32C0699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C412DB-CAEC-4BCA-B8E8-831F5E8AD436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,10 +134,10 @@
 modal wasn’t closing after form misinput</t>
   </si>
   <si>
-    <t>after implementing this, a bug where flash msg persists appeared</t>
-  </si>
-  <si>
     <t>Register, logout, and login has a flash bug, and its error msg needs revamp</t>
+  </si>
+  <si>
+    <t>fixed bug where flash mgs exists</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
@@ -729,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
tweaked UI for modals a bit
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C412DB-CAEC-4BCA-B8E8-831F5E8AD436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885CFEB0-79A8-4564-A951-0C6386A70F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Backend part remaining</t>
   </si>
   <si>
-    <t>Task 13:</t>
-  </si>
-  <si>
     <t>Task 14:</t>
   </si>
   <si>
@@ -124,20 +121,16 @@
     <t>Task 12 :Login Backend</t>
   </si>
   <si>
-    <t>02/15/2024</t>
-  </si>
-  <si>
-    <t>02/16/2024</t>
-  </si>
-  <si>
-    <t>not sure if this is complete yet, but it seems it is. Had an issue where 
-modal wasn’t closing after form misinput</t>
-  </si>
-  <si>
-    <t>Register, logout, and login has a flash bug, and its error msg needs revamp</t>
-  </si>
-  <si>
-    <t>fixed bug where flash mgs exists</t>
+    <t>02/21/2024</t>
+  </si>
+  <si>
+    <t>fixed bug where flash mgs exists, UI needs a few more polishing</t>
+  </si>
+  <si>
+    <t>modal wasn’t closing after form misinput bug fixed, UI needs a few more polishing</t>
+  </si>
+  <si>
+    <t>Task 13: Polish form sizes for different screens</t>
   </si>
 </sst>
 </file>
@@ -554,7 +547,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +613,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -637,7 +630,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -662,7 +655,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -673,7 +666,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -684,7 +677,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
@@ -697,47 +690,47 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>12</v>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -745,7 +738,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -753,7 +746,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
@@ -761,7 +754,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
@@ -769,7 +762,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -777,7 +770,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added column to projects table to distinguish project owner
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885CFEB0-79A8-4564-A951-0C6386A70F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2866C456-65E6-4CEB-AA67-A56A4712FACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -85,21 +85,6 @@
     <t>Backend part remaining</t>
   </si>
   <si>
-    <t>Task 14:</t>
-  </si>
-  <si>
-    <t>Task 15:</t>
-  </si>
-  <si>
-    <t>Task 16:</t>
-  </si>
-  <si>
-    <t>Task 17:</t>
-  </si>
-  <si>
-    <t>Task 18:</t>
-  </si>
-  <si>
     <t>Task 6: DB:Schema/ERD</t>
   </si>
   <si>
@@ -131,6 +116,24 @@
   </si>
   <si>
     <t>Task 13: Polish form sizes for different screens</t>
+  </si>
+  <si>
+    <t>Task 14: Projects Page Frontend</t>
+  </si>
+  <si>
+    <t>Task 15: Projects Cread (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 16: Projects Read (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 17: Projects Update (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 18: Projects Delete (CRUD)</t>
+  </si>
+  <si>
+    <t>02/22/2024</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +616,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -630,7 +633,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -655,7 +658,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -666,7 +669,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -677,7 +680,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
@@ -694,51 +697,54 @@
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -746,7 +752,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
@@ -754,7 +760,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
@@ -762,7 +768,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -770,7 +776,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted form field sizes, found a password overlapping layout bug
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2866C456-65E6-4CEB-AA67-A56A4712FACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485FE1AD-1A3C-41DC-B637-940DF42B6527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Task</t>
   </si>
@@ -115,9 +115,6 @@
     <t>modal wasn’t closing after form misinput bug fixed, UI needs a few more polishing</t>
   </si>
   <si>
-    <t>Task 13: Polish form sizes for different screens</t>
-  </si>
-  <si>
     <t>Task 14: Projects Page Frontend</t>
   </si>
   <si>
@@ -134,6 +131,63 @@
   </si>
   <si>
     <t>02/22/2024</t>
+  </si>
+  <si>
+    <t>Task 19:</t>
+  </si>
+  <si>
+    <t>Task 20:</t>
+  </si>
+  <si>
+    <t>Task 21:</t>
+  </si>
+  <si>
+    <t>Task 22:</t>
+  </si>
+  <si>
+    <t>Task 23:</t>
+  </si>
+  <si>
+    <t>Task 24:</t>
+  </si>
+  <si>
+    <t>Task 25:</t>
+  </si>
+  <si>
+    <t>Task 26:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 27: </t>
+  </si>
+  <si>
+    <t>Task 28:</t>
+  </si>
+  <si>
+    <t>Task 29:</t>
+  </si>
+  <si>
+    <t>Task 30:</t>
+  </si>
+  <si>
+    <t>Task 31:</t>
+  </si>
+  <si>
+    <t>Task 32:</t>
+  </si>
+  <si>
+    <t>Task 33:</t>
+  </si>
+  <si>
+    <t>Task 34:</t>
+  </si>
+  <si>
+    <t>Task 35:</t>
+  </si>
+  <si>
+    <t>Task 13: Modal form sizes for different screens</t>
+  </si>
+  <si>
+    <t>annoying bug where password interrups the layout of password form</t>
   </si>
 </sst>
 </file>
@@ -547,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,18 +787,21 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -752,7 +809,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
@@ -760,7 +817,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
@@ -768,7 +825,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -776,10 +833,95 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created route & template for projects page
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485FE1AD-1A3C-41DC-B637-940DF42B6527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF7FF40-56AE-4C3B-ABEF-B1391FD5F501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added task factory for each project and define props for projects page, to test further
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDAAFED-5C13-4E7A-A139-107192A15756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DCD860-58AD-4811-9518-7DC3D100A689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>Task</t>
   </si>
@@ -121,18 +121,9 @@
     <t>Task 16: Projects Read (CRUD)</t>
   </si>
   <si>
-    <t>Task 17: Projects Update (CRUD)</t>
-  </si>
-  <si>
-    <t>Task 18: Projects Delete (CRUD)</t>
-  </si>
-  <si>
     <t>02/22/2024</t>
   </si>
   <si>
-    <t>Task 19:</t>
-  </si>
-  <si>
     <t>Task 20:</t>
   </si>
   <si>
@@ -187,13 +178,25 @@
     <t>annoying bug where password interrups the layout of password form</t>
   </si>
   <si>
-    <t>Task 16: Projects Create (CRUD)</t>
-  </si>
-  <si>
-    <t>02/23/2024</t>
-  </si>
-  <si>
-    <t>Might need to reinvent. Will draw a another template this weekend</t>
+    <t>Template Sent to Self in Chat fb</t>
+  </si>
+  <si>
+    <t>Task 19: Projects Delete (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 18:Projects Update (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 17: Projects Create (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 15: Tasks Factory Seeder</t>
+  </si>
+  <si>
+    <t>02/24/2024</t>
+  </si>
+  <si>
+    <t>added db seeder, to test further</t>
   </si>
 </sst>
 </file>
@@ -610,20 +613,20 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,7 +643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -657,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -674,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -691,7 +694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -705,7 +708,7 @@
         <v>45414</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -716,7 +719,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -727,7 +730,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -738,7 +741,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -749,7 +752,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -763,7 +766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -777,7 +780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -791,21 +794,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -813,127 +816,130 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>50</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tasks Read Feature in projects page (CRUD)
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DCD860-58AD-4811-9518-7DC3D100A689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D90B1EA-59F5-4E9E-9EC3-DC950EE7C27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -124,18 +124,6 @@
     <t>02/22/2024</t>
   </si>
   <si>
-    <t>Task 20:</t>
-  </si>
-  <si>
-    <t>Task 21:</t>
-  </si>
-  <si>
-    <t>Task 22:</t>
-  </si>
-  <si>
-    <t>Task 23:</t>
-  </si>
-  <si>
     <t>Task 24:</t>
   </si>
   <si>
@@ -197,6 +185,24 @@
   </si>
   <si>
     <t>added db seeder, to test further</t>
+  </si>
+  <si>
+    <t>02/28/2024</t>
+  </si>
+  <si>
+    <t>Task 20: Tasks Read (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 21: Tasks Create (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 22: Tasks Update (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 23: Tasks Delete (CRUD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -613,7 +619,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,13 +802,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -816,130 +822,157 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>12</v>
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated projects page UI
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D90B1EA-59F5-4E9E-9EC3-DC950EE7C27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571EDB3E-95D7-4255-8E17-3066F66418C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -124,24 +124,6 @@
     <t>02/22/2024</t>
   </si>
   <si>
-    <t>Task 24:</t>
-  </si>
-  <si>
-    <t>Task 25:</t>
-  </si>
-  <si>
-    <t>Task 26:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task 27: </t>
-  </si>
-  <si>
-    <t>Task 28:</t>
-  </si>
-  <si>
-    <t>Task 29:</t>
-  </si>
-  <si>
     <t>Task 30:</t>
   </si>
   <si>
@@ -203,6 +185,24 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Task 24: Members Read (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 25: Members Create (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 26: Members Update (CRUD)</t>
+  </si>
+  <si>
+    <t>Task 27: Members Delete (CRUD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 29: </t>
+  </si>
+  <si>
+    <t>Task 28: Projects Page Frontend Polish (This Includes Projects, tasks, &amp; members)</t>
   </si>
 </sst>
 </file>
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -282,6 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,21 +619,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="64.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -666,7 +667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -683,7 +684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -700,7 +701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -714,7 +715,7 @@
         <v>45414</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -725,7 +726,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -736,7 +737,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -747,7 +748,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -758,7 +759,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -772,7 +773,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -786,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -800,21 +801,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -822,27 +823,27 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="D14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>49</v>
-      </c>
       <c r="D15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -850,129 +851,147 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="7">
+        <v>45415</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added projects button and fixed bug where selected project is not highlighted immediately
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571EDB3E-95D7-4255-8E17-3066F66418C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C72965-3B9F-40A3-88CA-D3BEA62B0FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>Task</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Task 28: Projects Page Frontend Polish (This Includes Projects, tasks, &amp; members)</t>
+  </si>
+  <si>
+    <t>created filters on vue frontend to implement this</t>
+  </si>
+  <si>
+    <t>created filters and.map on vue frontend to implement this</t>
   </si>
 </sst>
 </file>
@@ -620,7 +626,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,8 +891,11 @@
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
-        <v>44</v>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="7">
+        <v>45476</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,8 +929,11 @@
       <c r="A24" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>11</v>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -956,7 +968,7 @@
         <v>12</v>
       </c>
       <c r="D28" s="7">
-        <v>45415</v>
+        <v>45507</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed highlighted project color to cyan, and select projectedId is defaulted to 0 at start
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C72965-3B9F-40A3-88CA-D3BEA62B0FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50EA09F-38BA-4D19-A3E2-465C02508242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>Task</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>created filters and.map on vue frontend to implement this</t>
+  </si>
+  <si>
+    <t>03/14/2024</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,8 +867,11 @@
       <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>11</v>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completed backend for adding task, modal persisting bug persisting tho
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBC4A39-5B83-4BED-9798-2B43A40A0B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6500ADE-68AB-484D-A979-E4A2F91B689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,8 +908,8 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>11</v>
+      <c r="B21" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added a pen button for editing project
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6500ADE-68AB-484D-A979-E4A2F91B689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A952435-A699-4D9E-B1B8-6EB109D6F85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Task 27: Members Delete (CRUD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Task 29: </t>
-  </si>
-  <si>
     <t>Task 28: Projects Page Frontend Polish (This Includes Projects, tasks, &amp; members)</t>
   </si>
   <si>
@@ -212,6 +209,18 @@
   </si>
   <si>
     <t>03/14/2024</t>
+  </si>
+  <si>
+    <t>03/22/2024</t>
+  </si>
+  <si>
+    <t>this function is same as create, cant edit members, only create and delete</t>
+  </si>
+  <si>
+    <t>03/16/2024</t>
+  </si>
+  <si>
+    <t>Task 29: Storage (Local)</t>
   </si>
 </sst>
 </file>
@@ -629,20 +638,20 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="64.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -676,7 +685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -693,7 +702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -710,7 +719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -724,7 +733,7 @@
         <v>45414</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -735,7 +744,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -746,7 +755,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -757,7 +766,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -768,7 +777,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -782,7 +791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -796,7 +805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -810,7 +819,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -824,12 +833,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>12</v>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
@@ -838,7 +847,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -852,7 +861,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -863,18 +872,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>12</v>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -882,7 +891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -890,7 +899,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -898,21 +907,24 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="7">
         <v>45476</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -920,7 +932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -931,7 +943,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -939,26 +951,38 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -966,9 +990,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -977,37 +1001,37 @@
         <v>45507</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
fixed issue where editproject modal doesn't happen if there's no selected project
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A952435-A699-4D9E-B1B8-6EB109D6F85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D034B7-6152-4C61-A523-C1DB07C8FA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Task</t>
   </si>
@@ -121,12 +121,6 @@
     <t>Task 16: Projects Read (CRUD)</t>
   </si>
   <si>
-    <t>02/22/2024</t>
-  </si>
-  <si>
-    <t>Task 30:</t>
-  </si>
-  <si>
     <t>Task 31:</t>
   </si>
   <si>
@@ -142,9 +136,6 @@
     <t>Task 35:</t>
   </si>
   <si>
-    <t>Task 13: Modal form sizes for different screens</t>
-  </si>
-  <si>
     <t>annoying bug where password interrups the layout of password form</t>
   </si>
   <si>
@@ -199,9 +190,6 @@
     <t>Task 27: Members Delete (CRUD)</t>
   </si>
   <si>
-    <t>Task 28: Projects Page Frontend Polish (This Includes Projects, tasks, &amp; members)</t>
-  </si>
-  <si>
     <t>created filters on vue frontend to implement this</t>
   </si>
   <si>
@@ -220,7 +208,25 @@
     <t>03/16/2024</t>
   </si>
   <si>
-    <t>Task 29: Storage (Local)</t>
+    <t>03:27/2024</t>
+  </si>
+  <si>
+    <t>03/28/2024</t>
+  </si>
+  <si>
+    <t>this requires auth, alternative is v-if ownerid=user.id, only for project owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 30:  </t>
+  </si>
+  <si>
+    <t>Task 13: Projects Page Frontend Polish (This Includes Projects, tasks, &amp; members)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 29: </t>
+  </si>
+  <si>
+    <t>Task 28: Bug Fixes</t>
   </si>
 </sst>
 </file>
@@ -637,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,16 +827,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45385</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -841,24 +847,24 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -869,64 +875,70 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>11</v>
+        <v>35</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="7">
+        <v>51</v>
+      </c>
+      <c r="D20" s="3">
         <v>45476</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
@@ -934,65 +946,71 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -1003,37 +1021,37 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added deleteProject button, controller and route
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D034B7-6152-4C61-A523-C1DB07C8FA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E25E15D-D889-4D8C-8C53-ED4E96C84537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -644,7 +644,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added edit task modal
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E25E15D-D889-4D8C-8C53-ED4E96C84537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAA4C74-FCE5-4E0F-BA1B-E3AB8751FC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>Task</t>
   </si>
@@ -121,12 +121,6 @@
     <t>Task 16: Projects Read (CRUD)</t>
   </si>
   <si>
-    <t>Task 31:</t>
-  </si>
-  <si>
-    <t>Task 32:</t>
-  </si>
-  <si>
     <t>Task 33:</t>
   </si>
   <si>
@@ -211,22 +205,25 @@
     <t>03:27/2024</t>
   </si>
   <si>
-    <t>03/28/2024</t>
-  </si>
-  <si>
     <t>this requires auth, alternative is v-if ownerid=user.id, only for project owner</t>
   </si>
   <si>
-    <t xml:space="preserve">Task 30:  </t>
-  </si>
-  <si>
     <t>Task 13: Projects Page Frontend Polish (This Includes Projects, tasks, &amp; members)</t>
   </si>
   <si>
-    <t xml:space="preserve">Task 29: </t>
-  </si>
-  <si>
     <t>Task 28: Bug Fixes</t>
+  </si>
+  <si>
+    <t>Task 29: Frontend Polishing (Projects CRUD)</t>
+  </si>
+  <si>
+    <t>Task 30: Frontend Polishing (Tasks CRUD)</t>
+  </si>
+  <si>
+    <t>Task 31: Frontend Polishing (Members CRUD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 32: </t>
   </si>
 </sst>
 </file>
@@ -306,7 +303,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,13 +826,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3">
         <v>45385</v>
@@ -847,24 +846,24 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -875,51 +874,51 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>58</v>
+        <v>33</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45326</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" s="3">
         <v>45476</v>
@@ -927,18 +926,18 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
@@ -946,71 +945,71 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
         <v>52</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
         <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -1021,37 +1020,46 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
+      <c r="B30" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>61</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added delete task modal, controller, and route but this and edit task has bugs
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAA4C74-FCE5-4E0F-BA1B-E3AB8751FC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0104D68B-8061-45AC-AC36-2D2AC57887D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>Task</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Task 16: Projects Read (CRUD)</t>
   </si>
   <si>
-    <t>Task 33:</t>
-  </si>
-  <si>
     <t>Task 34:</t>
   </si>
   <si>
@@ -223,7 +220,10 @@
     <t>Task 31: Frontend Polishing (Members CRUD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Task 32: </t>
+    <t>Task 33:Bug Fix: clicking edit/delete button leads to wrong id</t>
+  </si>
+  <si>
+    <t>Task 32:Bug Fix: clicking project  edit button immediately leads to wrong id</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,13 +826,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="3">
         <v>45385</v>
@@ -846,24 +846,24 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -874,34 +874,34 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>6</v>
@@ -912,13 +912,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="3">
         <v>45476</v>
@@ -926,18 +926,18 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
@@ -945,71 +945,71 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>11</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>11</v>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>11</v>
@@ -1046,20 +1046,26 @@
       <c r="A32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added remove member modal (frontend only)
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0104D68B-8061-45AC-AC36-2D2AC57887D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E0FB31-33E8-49D8-BDCA-B0E1433F9C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>Task 23: Tasks Delete (CRUD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Task 24: Members Read (CRUD)</t>
@@ -642,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,7 +823,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -885,7 +882,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,7 +893,7 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -918,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="3">
         <v>45476</v>
@@ -932,84 +929,87 @@
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>11</v>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="7">
+        <v>45355</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="7">
+        <v>45355</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>11</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>11</v>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>11</v>
@@ -1044,26 +1044,32 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="7">
+        <v>45386</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="7">
+        <v>45386</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
added if condition so that only the project owner can edit a project
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E0FB31-33E8-49D8-BDCA-B0E1433F9C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF097690-89EA-44E0-9DFA-086D2CC44F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -121,12 +121,6 @@
     <t>Task 16: Projects Read (CRUD)</t>
   </si>
   <si>
-    <t>Task 34:</t>
-  </si>
-  <si>
-    <t>Task 35:</t>
-  </si>
-  <si>
     <t>annoying bug where password interrups the layout of password form</t>
   </si>
   <si>
@@ -221,6 +215,12 @@
   </si>
   <si>
     <t>Task 32:Bug Fix: clicking project  edit button immediately leads to wrong id</t>
+  </si>
+  <si>
+    <t>Task 34:Middleware for edit project (owner only)</t>
+  </si>
+  <si>
+    <t>Task 35: Middleware for remove/add member (owner only)</t>
   </si>
 </sst>
 </file>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,13 +823,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="3">
         <v>45385</v>
@@ -843,24 +843,24 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -871,34 +871,34 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>6</v>
@@ -909,13 +909,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3">
         <v>45476</v>
@@ -923,18 +923,18 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>6</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>6</v>
@@ -956,60 +956,63 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
         <v>48</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
         <v>48</v>
-      </c>
-      <c r="D25" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="D27" s="7">
+        <v>45416</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -1020,7 +1023,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>11</v>
@@ -1028,7 +1031,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>11</v>
@@ -1036,7 +1039,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>11</v>
@@ -1044,7 +1047,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>6</v>
@@ -1055,7 +1058,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>6</v>
@@ -1066,12 +1069,21 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>60</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="7">
+        <v>45416</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
projects page now only shows projects the current user is involved
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1B55E0-5CB3-4D5A-A448-B81263C2FB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF37B8C-F7B3-426B-AAFE-74DD08896495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>Task</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Task 37: Projects page revamp</t>
+  </si>
+  <si>
+    <t>Task 38: Manage project page</t>
   </si>
 </sst>
 </file>
@@ -652,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1120,6 +1123,9 @@
       <c r="A36" t="s">
         <v>64</v>
       </c>
+      <c r="B36" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="D36" t="s">
         <v>65</v>
       </c>
@@ -1127,6 +1133,17 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>66</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added screen size conditions for selectedProject section
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF37B8C-F7B3-426B-AAFE-74DD08896495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8A83D6-E0B0-4C03-A23F-D2A39CA0B1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -321,6 +321,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,20 +659,20 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="84" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -705,7 +706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -722,7 +723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -739,7 +740,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -753,7 +754,7 @@
         <v>45414</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -764,7 +765,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -775,7 +776,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -786,7 +787,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -797,7 +798,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -811,7 +812,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -825,7 +826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -839,7 +840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -853,7 +854,7 @@
         <v>45385</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -867,7 +868,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -881,7 +882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -892,7 +893,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -903,7 +904,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -914,7 +915,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -925,7 +926,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -939,7 +940,7 @@
         <v>45476</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -950,7 +951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -961,7 +962,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -972,7 +973,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -986,7 +987,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>45507</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>45386</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>45386</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -1138,12 +1139,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>11</v>
+      <c r="B38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="8">
+        <v>45509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added truncate and whitespace to projectnavbar components
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8A83D6-E0B0-4C03-A23F-D2A39CA0B1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD569CB0-ACC2-4D55-ABCF-EA4D3FBC5C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
   <si>
     <t>Task</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>Task 38: Manage project page</t>
+  </si>
+  <si>
+    <t>Task 39: Manage project page revamp</t>
   </si>
 </sst>
 </file>
@@ -656,23 +659,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="84" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -706,7 +709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -723,7 +726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -740,7 +743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -754,7 +757,7 @@
         <v>45414</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -765,7 +768,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -776,7 +779,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -787,7 +790,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -798,7 +801,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -812,7 +815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -826,7 +829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -840,7 +843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -854,7 +857,7 @@
         <v>45385</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -868,7 +871,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -882,7 +885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -893,7 +896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -904,7 +907,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -915,7 +918,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -926,7 +929,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -940,7 +943,7 @@
         <v>45476</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -951,7 +954,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -962,7 +965,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -973,7 +976,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -987,7 +990,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1029,7 +1032,7 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>45507</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>45386</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>45386</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -1148,6 +1151,17 @@
       </c>
       <c r="D38" s="8">
         <v>45509</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="8">
+        <v>45540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revamped add member to project page and fixed project page not loading if there's no logged in user
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD569CB0-ACC2-4D55-ABCF-EA4D3FBC5C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B37100C-6818-4381-9433-838B8379FD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
   <si>
     <t>Task</t>
   </si>
@@ -242,6 +242,15 @@
   </si>
   <si>
     <t>Task 39: Manage project page revamp</t>
+  </si>
+  <si>
+    <t>05/14/2024</t>
+  </si>
+  <si>
+    <t>added an optional tag in projectcontroller's $currentUserId</t>
+  </si>
+  <si>
+    <t>Task 40: Condition project page add buttons only if there's logged in user</t>
   </si>
 </sst>
 </file>
@@ -659,23 +668,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="84" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -709,7 +718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -726,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -743,7 +752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -757,7 +766,7 @@
         <v>45414</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -768,7 +777,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -779,7 +788,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -790,7 +799,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -801,7 +810,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -815,7 +824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -829,7 +838,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -843,7 +852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -857,7 +866,7 @@
         <v>45385</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -871,7 +880,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -885,7 +894,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -896,7 +905,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -907,7 +916,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -918,7 +927,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -929,7 +938,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -943,7 +952,7 @@
         <v>45476</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -954,7 +963,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -965,7 +974,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -976,7 +985,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -990,7 +999,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1032,7 +1041,7 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1043,7 +1052,7 @@
         <v>45507</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1051,7 +1060,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1059,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1067,7 +1076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1081,7 +1090,7 @@
         <v>45386</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1095,7 +1104,7 @@
         <v>45386</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -1109,7 +1118,7 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -1123,26 +1132,32 @@
         <v>45416</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>11</v>
+      <c r="B36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
       </c>
       <c r="D36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -1153,7 +1168,7 @@
         <v>45509</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -1162,6 +1177,14 @@
       </c>
       <c r="D39" s="8">
         <v>45540</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added error message to addprojectmodal
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B37100C-6818-4381-9433-838B8379FD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05777767-6673-48FD-A4CF-454E65A65A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>Task</t>
   </si>
@@ -251,6 +251,24 @@
   </si>
   <si>
     <t>Task 40: Condition project page add buttons only if there's logged in user</t>
+  </si>
+  <si>
+    <t>05/21/2024</t>
+  </si>
+  <si>
+    <t>05/22/2024</t>
+  </si>
+  <si>
+    <t>05/24/2024</t>
+  </si>
+  <si>
+    <t>05/27/2024</t>
+  </si>
+  <si>
+    <t>Task 41: Inculcate error texts in forms, add project will be ur basis since it works</t>
+  </si>
+  <si>
+    <t>Task 42: Fix bug not closing modal upon form completion</t>
   </si>
 </sst>
 </file>
@@ -668,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A872B34D-1F35-44FD-9489-A6BD8FAF6868}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,14 +874,14 @@
       <c r="A13" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3">
-        <v>45385</v>
+      <c r="D13" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1056,24 +1074,33 @@
       <c r="A29" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>11</v>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>11</v>
+      <c r="B30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>11</v>
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,6 +1212,16 @@
       </c>
       <c r="B40" s="5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added form errors and fixed on addtask modal not closing onSuccess
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\gilvin-todo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05777767-6673-48FD-A4CF-454E65A65A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B59726-55ED-48C3-943A-9F4373F873FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC17ABA-271A-46DD-933C-A0E8F8C86631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
   <si>
     <t>Task</t>
   </si>
@@ -268,7 +268,7 @@
     <t>Task 41: Inculcate error texts in forms, add project will be ur basis since it works</t>
   </si>
   <si>
-    <t>Task 42: Fix bug not closing modal upon form completion</t>
+    <t>Task 42: Fix bug not closing modal upon form completion, add project will also be ur basis since it works</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,18 +1210,27 @@
       <c r="A40" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>11</v>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>76</v>
       </c>
+      <c r="B41" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>77</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>